<commit_message>
Updated backend to correctly append emails to Excel
</commit_message>
<xml_diff>
--- a/server/subscribers.xlsx
+++ b/server/subscribers.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011" filterPrivacy="true"/>
   <sheets>
     <sheet name="Subscribers" sheetId="1" r:id="rId1"/>
   </sheets>
@@ -399,7 +399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -412,18 +412,15 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>avinash@gmail.com</v>
-      </c>
-      <c r="B2" t="str">
-        <v>10/30/2025, 5:07:39 PM</v>
+        <v>as@gmail.com</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>avi@gmail.com</v>
+        <v>yadav@gmail.com</v>
       </c>
       <c r="B3" t="str">
-        <v>10/30/2025, 5:30:36 PM</v>
+        <v>11/1/2025, 8:50:26 PM</v>
       </c>
     </row>
   </sheetData>

</xml_diff>